<commit_message>
sửa lại template của monitor store image
</commit_message>
<xml_diff>
--- a/DMS/Templates/Monitor_Store_Image.xlsx
+++ b/DMS/Templates/Monitor_Store_Image.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tai lieu du an\Rang Dong\DMS\Xuat bao cao - Giam sat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>CÔNG TY CỔ PHẦN BÓNG ĐÈN PHÍCH NƯỚC RẠNG ĐÔNG</t>
   </si>
@@ -41,12 +41,6 @@
     <t>Tên nhân viên</t>
   </si>
   <si>
-    <t>NV001</t>
-  </si>
-  <si>
-    <t>Nguyễn Văn Anh</t>
-  </si>
-  <si>
     <t>Hình ảnh</t>
   </si>
   <si>
@@ -59,34 +53,34 @@
     <t>Đến ngày</t>
   </si>
   <si>
-    <t>{đến ngày}</t>
-  </si>
-  <si>
-    <t>{từ ngày}</t>
-  </si>
-  <si>
-    <t>Khách hàng</t>
-  </si>
-  <si>
-    <t>20/05/2020</t>
-  </si>
-  <si>
-    <t>21/05/2021</t>
-  </si>
-  <si>
-    <t>22/05/2022</t>
-  </si>
-  <si>
-    <t>Cửa hàng Hoàng Hà</t>
-  </si>
-  <si>
-    <t>Cửa hàng Mai Lan</t>
-  </si>
-  <si>
-    <t>Cửa hàng Đồng Tiến</t>
-  </si>
-  <si>
-    <t>{Đơn vị quản lý}</t>
+    <t>{{Start}}</t>
+  </si>
+  <si>
+    <t>{{End}}</t>
+  </si>
+  <si>
+    <t>{{MonitorStoreImages.OrganizationName}}</t>
+  </si>
+  <si>
+    <t>{{MonitorStoreImages.SaleEmployees.Username}}</t>
+  </si>
+  <si>
+    <t>{{MonitorStoreImages.SaleEmployees.DisplayName}}</t>
+  </si>
+  <si>
+    <t>{{MonitorStoreImages.SaleEmployees.StoreCheckings.STT}}</t>
+  </si>
+  <si>
+    <t>{{MonitorStoreImages.SaleEmployees.StoreCheckings.DateDisplay}}</t>
+  </si>
+  <si>
+    <t>{{MonitorStoreImages.SaleEmployees.StoreCheckings.StoreName}}</t>
+  </si>
+  <si>
+    <t>Đại lý</t>
+  </si>
+  <si>
+    <t>{{MonitorStoreImages.SaleEmployees.StoreCheckings.ImageCounter}}</t>
   </si>
 </sst>
 </file>
@@ -145,7 +139,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -205,54 +199,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -274,23 +230,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -572,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,143 +537,77 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>7</v>
+      <c r="E7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="12"/>
+      <c r="A8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
-        <v>1</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="A9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
-        <v>2</v>
-      </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="6" t="s">
+      <c r="B9" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="6">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
-        <v>3</v>
-      </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="1">
     <mergeCell ref="A8:F8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>